<commit_message>
Added drill bit information to processes.
</commit_message>
<xml_diff>
--- a/03 BOM/Barrier Conveyor BOM.xlsx
+++ b/03 BOM/Barrier Conveyor BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Balsamo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B76D6D-FF73-4085-BFDE-413982A7C1A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393A3D36-C1A6-4C4A-B231-B57A3093B2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flattened BOM - Barrier Conveyo" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="410">
   <si>
     <t>Easy</t>
   </si>
@@ -1267,6 +1267,9 @@
   </si>
   <si>
     <t>0044918</t>
+  </si>
+  <si>
+    <t>5/8" Diam. or greater drill bit (aluminum)</t>
   </si>
 </sst>
 </file>
@@ -1475,7 +1478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1577,16 +1580,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1603,6 +1597,22 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1849,9 +1859,9 @@
   </sheetPr>
   <dimension ref="A1:Q189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1860,7 +1870,7 @@
     <col min="2" max="2" width="88.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" style="77" customWidth="1"/>
+    <col min="5" max="6" width="7.28515625" style="72" customWidth="1"/>
     <col min="7" max="7" width="4.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="10" width="21.5703125" customWidth="1"/>
@@ -1930,14 +1940,14 @@
       <c r="B2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="73" t="s">
         <v>391</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="3">
         <v>2</v>
       </c>
@@ -1947,7 +1957,7 @@
       <c r="I2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K2" s="20"/>
@@ -1970,14 +1980,14 @@
       <c r="B3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="74" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="3">
         <v>20</v>
       </c>
@@ -1987,7 +1997,7 @@
       <c r="I3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="70" t="s">
         <v>69</v>
       </c>
       <c r="K3" s="18" t="b">
@@ -2014,14 +2024,14 @@
       <c r="B4" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="73" t="s">
         <v>384</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
       <c r="G4" s="3">
         <v>1</v>
       </c>
@@ -2031,7 +2041,7 @@
       <c r="I4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="J4" s="70" t="s">
         <v>78</v>
       </c>
       <c r="K4" s="18" t="b">
@@ -2057,14 +2067,14 @@
       <c r="B5" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="74" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="3">
         <v>1</v>
       </c>
@@ -2074,7 +2084,7 @@
       <c r="I5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="70" t="s">
         <v>85</v>
       </c>
       <c r="K5" s="18" t="b">
@@ -2101,14 +2111,14 @@
       <c r="B6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="73" t="s">
         <v>385</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="3">
         <v>1</v>
       </c>
@@ -2118,7 +2128,7 @@
       <c r="I6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="70" t="s">
         <v>90</v>
       </c>
       <c r="K6" s="18" t="b">
@@ -2145,14 +2155,14 @@
       <c r="B7" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="74" t="s">
         <v>95</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3">
         <v>4</v>
       </c>
@@ -2162,7 +2172,7 @@
       <c r="I7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="75" t="s">
+      <c r="J7" s="70" t="s">
         <v>98</v>
       </c>
       <c r="K7" s="18" t="b">
@@ -2188,16 +2198,16 @@
       <c r="B8" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="73" t="s">
         <v>398</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F8" s="76"/>
+      <c r="F8" s="71"/>
       <c r="G8" s="3">
         <v>4</v>
       </c>
@@ -2207,7 +2217,7 @@
       <c r="I8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K8" s="20"/>
@@ -2230,14 +2240,14 @@
       <c r="B9" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="73" t="s">
         <v>395</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
       <c r="G9" s="3">
         <v>2</v>
       </c>
@@ -2247,7 +2257,7 @@
       <c r="I9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="75" t="s">
+      <c r="J9" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K9" s="20"/>
@@ -2270,14 +2280,14 @@
       <c r="B10" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="73" t="s">
         <v>396</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="3">
         <v>4</v>
       </c>
@@ -2287,7 +2297,7 @@
       <c r="I10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K10" s="20"/>
@@ -2310,16 +2320,16 @@
       <c r="B11" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="73" t="s">
         <v>397</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F11" s="76"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="3">
         <v>1</v>
       </c>
@@ -2329,7 +2339,7 @@
       <c r="I11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K11" s="20"/>
@@ -2352,14 +2362,14 @@
       <c r="B12" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="73" t="s">
         <v>386</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
       <c r="G12" s="3">
         <v>1</v>
       </c>
@@ -2369,7 +2379,7 @@
       <c r="I12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="70" t="s">
         <v>122</v>
       </c>
       <c r="K12" s="18" t="b">
@@ -2395,14 +2405,14 @@
       <c r="B13" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="74" t="s">
         <v>119</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="3">
         <v>4</v>
       </c>
@@ -2412,7 +2422,7 @@
       <c r="I13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="75" t="s">
+      <c r="J13" s="70" t="s">
         <v>121</v>
       </c>
       <c r="K13" s="18" t="b">
@@ -2441,14 +2451,14 @@
       <c r="B14" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="74" t="s">
         <v>136</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76" t="s">
+      <c r="E14" s="71"/>
+      <c r="F14" s="71" t="s">
         <v>383</v>
       </c>
       <c r="G14" s="3">
@@ -2460,7 +2470,7 @@
       <c r="I14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="75" t="s">
+      <c r="J14" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K14" s="20"/>
@@ -2483,14 +2493,14 @@
       <c r="B15" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="73" t="s">
         <v>387</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="3">
         <v>8</v>
       </c>
@@ -2500,7 +2510,7 @@
       <c r="I15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J15" s="75" t="s">
+      <c r="J15" s="70" t="s">
         <v>144</v>
       </c>
       <c r="K15" s="18" t="b">
@@ -2527,14 +2537,14 @@
       <c r="B16" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="79" t="s">
+      <c r="C16" s="74" t="s">
         <v>149</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
       <c r="G16" s="3">
         <v>2</v>
       </c>
@@ -2544,7 +2554,7 @@
       <c r="I16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J16" s="75" t="s">
+      <c r="J16" s="70" t="s">
         <v>151</v>
       </c>
       <c r="K16" s="18" t="b">
@@ -2570,14 +2580,14 @@
       <c r="B17" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="75" t="s">
         <v>393</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
       <c r="G17" s="3">
         <v>8</v>
       </c>
@@ -2587,7 +2597,7 @@
       <c r="I17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="75" t="s">
+      <c r="J17" s="70" t="s">
         <v>156</v>
       </c>
       <c r="K17" s="18" t="b">
@@ -2614,16 +2624,16 @@
       <c r="B18" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="73" t="s">
         <v>392</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="76" t="s">
+      <c r="E18" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F18" s="76"/>
+      <c r="F18" s="71"/>
       <c r="G18" s="3">
         <v>4</v>
       </c>
@@ -2633,7 +2643,7 @@
       <c r="I18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="75" t="s">
+      <c r="J18" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K18" s="20"/>
@@ -2656,16 +2666,16 @@
       <c r="B19" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="74" t="s">
         <v>163</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="76" t="s">
+      <c r="E19" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F19" s="76"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="3">
         <v>8</v>
       </c>
@@ -2675,7 +2685,7 @@
       <c r="I19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="75" t="s">
+      <c r="J19" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K19" s="20"/>
@@ -2698,14 +2708,14 @@
       <c r="B20" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="74" t="s">
         <v>166</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
       <c r="G20" s="3">
         <v>1</v>
       </c>
@@ -2715,7 +2725,7 @@
       <c r="I20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J20" s="75" t="s">
+      <c r="J20" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K20" s="18" t="b">
@@ -2741,14 +2751,14 @@
       <c r="B21" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="74" t="s">
         <v>170</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="3">
         <v>3</v>
       </c>
@@ -2758,7 +2768,7 @@
       <c r="I21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="75" t="s">
+      <c r="J21" s="70" t="s">
         <v>171</v>
       </c>
       <c r="K21" s="18" t="b">
@@ -2784,14 +2794,14 @@
       <c r="B22" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="74" t="s">
         <v>174</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
       <c r="G22" s="3">
         <v>4</v>
       </c>
@@ -2801,7 +2811,7 @@
       <c r="I22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="75" t="s">
+      <c r="J22" s="70" t="s">
         <v>175</v>
       </c>
       <c r="K22" s="18" t="b">
@@ -2827,14 +2837,14 @@
       <c r="B23" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="74" t="s">
         <v>178</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
       <c r="G23" s="3">
         <v>12</v>
       </c>
@@ -2844,7 +2854,7 @@
       <c r="I23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="75" t="s">
+      <c r="J23" s="70" t="s">
         <v>180</v>
       </c>
       <c r="K23" s="18" t="b">
@@ -2870,14 +2880,14 @@
       <c r="B24" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="78" t="s">
+      <c r="C24" s="73" t="s">
         <v>388</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
       <c r="G24" s="3">
         <v>2</v>
       </c>
@@ -2887,7 +2897,7 @@
       <c r="I24" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J24" s="75" t="s">
+      <c r="J24" s="70" t="s">
         <v>111</v>
       </c>
       <c r="K24" s="18" t="b">
@@ -2916,16 +2926,16 @@
       <c r="B25" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C25" s="79" t="s">
+      <c r="C25" s="74" t="s">
         <v>182</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E25" s="76" t="s">
+      <c r="E25" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F25" s="76"/>
+      <c r="F25" s="71"/>
       <c r="G25" s="3">
         <v>2</v>
       </c>
@@ -2935,7 +2945,7 @@
       <c r="I25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="75" t="s">
+      <c r="J25" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K25" s="20"/>
@@ -2958,16 +2968,16 @@
       <c r="B26" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="73" t="s">
         <v>399</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E26" s="76" t="s">
+      <c r="E26" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F26" s="76"/>
+      <c r="F26" s="71"/>
       <c r="G26" s="3">
         <v>1</v>
       </c>
@@ -2977,7 +2987,7 @@
       <c r="I26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="75" t="s">
+      <c r="J26" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K26" s="20"/>
@@ -3000,16 +3010,16 @@
       <c r="B27" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="73" t="s">
         <v>400</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="76" t="s">
+      <c r="E27" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F27" s="76"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="3">
         <v>1</v>
       </c>
@@ -3019,7 +3029,7 @@
       <c r="I27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J27" s="75" t="s">
+      <c r="J27" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="20"/>
@@ -3042,16 +3052,16 @@
       <c r="B28" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="73" t="s">
         <v>402</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F28" s="76"/>
+      <c r="F28" s="71"/>
       <c r="G28" s="3">
         <v>2</v>
       </c>
@@ -3061,7 +3071,7 @@
       <c r="I28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J28" s="75" t="s">
+      <c r="J28" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K28" s="20"/>
@@ -3085,16 +3095,16 @@
       <c r="B29" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C29" s="78" t="s">
+      <c r="C29" s="73" t="s">
         <v>401</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E29" s="76" t="s">
+      <c r="E29" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F29" s="76"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="3">
         <v>2</v>
       </c>
@@ -3104,7 +3114,7 @@
       <c r="I29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J29" s="75" t="s">
+      <c r="J29" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K29" s="20"/>
@@ -3130,16 +3140,16 @@
       <c r="B30" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C30" s="78" t="s">
+      <c r="C30" s="73" t="s">
         <v>403</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="76" t="s">
+      <c r="E30" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F30" s="76"/>
+      <c r="F30" s="71"/>
       <c r="G30" s="3">
         <v>4</v>
       </c>
@@ -3149,7 +3159,7 @@
       <c r="I30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J30" s="75" t="s">
+      <c r="J30" s="70" t="s">
         <v>54</v>
       </c>
       <c r="K30" s="20"/>
@@ -3172,16 +3182,16 @@
       <c r="B31" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C31" s="73" t="s">
         <v>404</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E31" s="76" t="s">
+      <c r="E31" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F31" s="76" t="s">
+      <c r="F31" s="71" t="s">
         <v>383</v>
       </c>
       <c r="G31" s="3">
@@ -3193,7 +3203,7 @@
       <c r="I31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J31" s="75" t="s">
+      <c r="J31" s="70" t="s">
         <v>196</v>
       </c>
       <c r="K31" s="18" t="b">
@@ -3219,14 +3229,14 @@
       <c r="B32" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="C32" s="79" t="s">
+      <c r="C32" s="74" t="s">
         <v>199</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
       <c r="G32" s="3">
         <v>2</v>
       </c>
@@ -3236,7 +3246,7 @@
       <c r="I32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J32" s="75" t="s">
+      <c r="J32" s="70" t="s">
         <v>200</v>
       </c>
       <c r="K32" s="18" t="b">
@@ -3263,14 +3273,14 @@
       <c r="B33" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C33" s="73" t="s">
         <v>202</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
       <c r="G33" s="3">
         <f>18+23</f>
         <v>41</v>
@@ -3281,7 +3291,7 @@
       <c r="I33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J33" s="75" t="s">
+      <c r="J33" s="70" t="s">
         <v>203</v>
       </c>
       <c r="K33" s="18" t="b">
@@ -3308,14 +3318,14 @@
       <c r="B34" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="81" t="s">
+      <c r="C34" s="76" t="s">
         <v>206</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
       <c r="G34" s="5">
         <v>4</v>
       </c>
@@ -3325,7 +3335,7 @@
       <c r="I34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J34" s="75" t="s">
+      <c r="J34" s="70" t="s">
         <v>207</v>
       </c>
       <c r="K34" s="18" t="b">
@@ -3352,14 +3362,14 @@
       <c r="B35" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C35" s="78" t="s">
+      <c r="C35" s="73" t="s">
         <v>389</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
       <c r="G35" s="3">
         <v>20</v>
       </c>
@@ -3369,7 +3379,7 @@
       <c r="I35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J35" s="75" t="s">
+      <c r="J35" s="70" t="s">
         <v>210</v>
       </c>
       <c r="K35" s="18" t="b">
@@ -3396,14 +3406,14 @@
       <c r="B36" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="78" t="s">
+      <c r="C36" s="73" t="s">
         <v>390</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
       <c r="G36" s="3">
         <v>46</v>
       </c>
@@ -3413,7 +3423,7 @@
       <c r="I36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J36" s="75" t="s">
+      <c r="J36" s="70" t="s">
         <v>212</v>
       </c>
       <c r="K36" s="18" t="b">
@@ -3440,14 +3450,14 @@
       <c r="B37" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="74" t="s">
         <v>214</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
       <c r="G37" s="3">
         <v>12</v>
       </c>
@@ -3457,7 +3467,7 @@
       <c r="I37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J37" s="75" t="s">
+      <c r="J37" s="70" t="s">
         <v>215</v>
       </c>
       <c r="K37" s="18" t="b">
@@ -3484,14 +3494,14 @@
       <c r="B38" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C38" s="78" t="s">
+      <c r="C38" s="73" t="s">
         <v>405</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
       <c r="G38" s="3">
         <v>3</v>
       </c>
@@ -3501,7 +3511,7 @@
       <c r="I38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J38" s="75" t="s">
+      <c r="J38" s="70" t="s">
         <v>60</v>
       </c>
       <c r="K38" s="18" t="b">
@@ -3527,14 +3537,14 @@
       <c r="B39" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C39" s="74" t="s">
         <v>218</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
       <c r="G39" s="3">
         <v>2</v>
       </c>
@@ -3544,7 +3554,7 @@
       <c r="I39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J39" s="75" t="s">
+      <c r="J39" s="70" t="s">
         <v>60</v>
       </c>
       <c r="K39" s="18" t="b">
@@ -3572,14 +3582,14 @@
       <c r="B40" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C40" s="78" t="s">
+      <c r="C40" s="73" t="s">
         <v>406</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
       <c r="G40" s="3">
         <v>4</v>
       </c>
@@ -3589,7 +3599,7 @@
       <c r="I40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J40" s="75" t="s">
+      <c r="J40" s="70" t="s">
         <v>60</v>
       </c>
       <c r="K40" s="18" t="b">
@@ -3617,14 +3627,14 @@
       <c r="B41" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="C41" s="79" t="s">
+      <c r="C41" s="74" t="s">
         <v>222</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
       <c r="G41" s="3">
         <v>2</v>
       </c>
@@ -3634,7 +3644,7 @@
       <c r="I41" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="75" t="s">
+      <c r="J41" s="70" t="s">
         <v>223</v>
       </c>
       <c r="K41" s="18" t="b">
@@ -3664,14 +3674,14 @@
       <c r="B42" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="73" t="s">
         <v>407</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
       <c r="G42" s="3">
         <v>2</v>
       </c>
@@ -3681,7 +3691,7 @@
       <c r="I42" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J42" s="75" t="s">
+      <c r="J42" s="70" t="s">
         <v>223</v>
       </c>
       <c r="K42" s="18" t="b">
@@ -3710,14 +3720,14 @@
       <c r="B43" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="78" t="s">
+      <c r="C43" s="73" t="s">
         <v>408</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
       <c r="G43" s="3">
         <v>1</v>
       </c>
@@ -3727,7 +3737,7 @@
       <c r="I43" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J43" s="75" t="s">
+      <c r="J43" s="70" t="s">
         <v>145</v>
       </c>
       <c r="K43" s="18" t="b">
@@ -3756,14 +3766,14 @@
       <c r="B44" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="C44" s="79" t="s">
+      <c r="C44" s="74" t="s">
         <v>226</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
       <c r="G44" s="3">
         <v>2</v>
       </c>
@@ -3773,7 +3783,7 @@
       <c r="I44" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J44" s="75" t="s">
+      <c r="J44" s="70" t="s">
         <v>227</v>
       </c>
       <c r="K44" s="18" t="b">
@@ -3800,14 +3810,14 @@
       <c r="B45" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="C45" s="79" t="s">
+      <c r="C45" s="74" t="s">
         <v>230</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
       <c r="G45" s="3">
         <v>2</v>
       </c>
@@ -3817,7 +3827,7 @@
       <c r="I45" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J45" s="75" t="s">
+      <c r="J45" s="70" t="s">
         <v>231</v>
       </c>
       <c r="K45" s="18" t="b">
@@ -3841,14 +3851,14 @@
       <c r="B46" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="74" t="s">
         <v>233</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
       <c r="G46" s="3">
         <v>3</v>
       </c>
@@ -3858,7 +3868,7 @@
       <c r="I46" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J46" s="75" t="s">
+      <c r="J46" s="70" t="s">
         <v>234</v>
       </c>
       <c r="K46" s="18" t="b">
@@ -3885,14 +3895,14 @@
       <c r="B47" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="C47" s="79" t="s">
+      <c r="C47" s="74" t="s">
         <v>237</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="76"/>
-      <c r="F47" s="76"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
       <c r="G47" s="3">
         <v>1</v>
       </c>
@@ -3902,7 +3912,7 @@
       <c r="I47" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J47" s="75" t="s">
+      <c r="J47" s="70" t="s">
         <v>238</v>
       </c>
       <c r="K47" s="18" t="b">
@@ -3926,14 +3936,14 @@
       <c r="B48" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C48" s="79" t="s">
+      <c r="C48" s="74" t="s">
         <v>240</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="76"/>
-      <c r="F48" s="76"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
       <c r="G48" s="59">
         <v>4</v>
       </c>
@@ -3943,7 +3953,7 @@
       <c r="I48" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J48" s="75" t="s">
+      <c r="J48" s="70" t="s">
         <v>241</v>
       </c>
       <c r="K48" s="18" t="b">
@@ -3967,21 +3977,21 @@
       <c r="B49" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="C49" s="82" t="s">
+      <c r="C49" s="77" t="s">
         <v>243</v>
       </c>
       <c r="D49" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
       <c r="G49" s="59">
         <v>1</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J49" s="75" t="s">
+      <c r="J49" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K49" s="20"/>
@@ -4001,21 +4011,21 @@
       <c r="B50" s="60" t="s">
         <v>246</v>
       </c>
-      <c r="C50" s="82" t="s">
+      <c r="C50" s="77" t="s">
         <v>247</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E50" s="76"/>
-      <c r="F50" s="76"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
       <c r="G50" s="59">
         <v>1</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J50" s="75" t="s">
+      <c r="J50" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K50" s="20"/>
@@ -4037,21 +4047,21 @@
       <c r="B51" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="82" t="s">
+      <c r="C51" s="77" t="s">
         <v>249</v>
       </c>
       <c r="D51" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E51" s="76"/>
-      <c r="F51" s="76"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
       <c r="G51" s="59">
         <v>1</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J51" s="75" t="s">
+      <c r="J51" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K51" s="20"/>
@@ -4073,21 +4083,21 @@
       <c r="B52" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C52" s="79" t="s">
+      <c r="C52" s="74" t="s">
         <v>252</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
       <c r="G52" s="59">
         <v>1</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J52" s="75" t="s">
+      <c r="J52" s="70" t="s">
         <v>254</v>
       </c>
       <c r="K52" s="18" t="b">
@@ -4110,21 +4120,21 @@
       <c r="B53" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C53" s="79" t="s">
+      <c r="C53" s="74" t="s">
         <v>258</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E53" s="76"/>
-      <c r="F53" s="76"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
       <c r="G53" s="59">
         <v>1</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J53" s="75" t="s">
+      <c r="J53" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K53" s="18" t="b">
@@ -4144,21 +4154,21 @@
       <c r="B54" s="61" t="s">
         <v>261</v>
       </c>
-      <c r="C54" s="83" t="s">
+      <c r="C54" s="78" t="s">
         <v>262</v>
       </c>
       <c r="D54" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
       <c r="G54" s="59">
         <v>1</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J54" s="75" t="s">
+      <c r="J54" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K54" s="20"/>
@@ -4178,14 +4188,14 @@
       <c r="B55" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C55" s="79" t="s">
+      <c r="C55" s="74" t="s">
         <v>264</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
       <c r="G55" s="59">
         <v>1</v>
       </c>
@@ -4195,7 +4205,7 @@
       <c r="I55" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="J55" s="75" t="s">
+      <c r="J55" s="70" t="s">
         <v>267</v>
       </c>
       <c r="K55" s="18" t="b">
@@ -4221,21 +4231,21 @@
       <c r="B56" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C56" s="79" t="s">
+      <c r="C56" s="74" t="s">
         <v>270</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
       <c r="G56" s="59">
         <v>1</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J56" s="75" t="s">
+      <c r="J56" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K56" s="18" t="b">
@@ -4255,21 +4265,21 @@
       <c r="B57" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C57" s="79" t="s">
+      <c r="C57" s="74" t="s">
         <v>274</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="76"/>
-      <c r="F57" s="76"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="71"/>
       <c r="G57" s="59">
         <v>1</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J57" s="75" t="s">
+      <c r="J57" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K57" s="18" t="b">
@@ -4287,21 +4297,21 @@
       <c r="B58" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C58" s="79" t="s">
+      <c r="C58" s="74" t="s">
         <v>276</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="E58" s="76"/>
-      <c r="F58" s="76"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="71"/>
       <c r="G58" s="59">
         <v>1</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J58" s="75" t="s">
+      <c r="J58" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K58" s="18" t="b">
@@ -4321,21 +4331,21 @@
       <c r="B59" s="60" t="s">
         <v>277</v>
       </c>
-      <c r="C59" s="82" t="s">
+      <c r="C59" s="77" t="s">
         <v>278</v>
       </c>
       <c r="D59" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E59" s="76"/>
-      <c r="F59" s="76"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
       <c r="G59" s="59">
         <v>1</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J59" s="75" t="s">
+      <c r="J59" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K59" s="20"/>
@@ -4355,21 +4365,21 @@
       <c r="B60" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C60" s="79" t="s">
+      <c r="C60" s="74" t="s">
         <v>280</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
       <c r="G60" s="59">
         <v>1</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J60" s="75" t="s">
+      <c r="J60" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K60" s="18" t="b">
@@ -4387,21 +4397,21 @@
       <c r="B61" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C61" s="79" t="s">
+      <c r="C61" s="74" t="s">
         <v>282</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
       <c r="G61" s="59">
         <v>1</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J61" s="75" t="s">
+      <c r="J61" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K61" s="18" t="b">
@@ -4421,21 +4431,21 @@
       <c r="B62" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C62" s="79" t="s">
+      <c r="C62" s="74" t="s">
         <v>284</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E62" s="76"/>
-      <c r="F62" s="76"/>
+      <c r="E62" s="71"/>
+      <c r="F62" s="71"/>
       <c r="G62" s="59">
         <v>1</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J62" s="75" t="s">
+      <c r="J62" s="70" t="s">
         <v>382</v>
       </c>
       <c r="K62" s="18" t="b">
@@ -4455,21 +4465,21 @@
       <c r="B63" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C63" s="79" t="s">
+      <c r="C63" s="74" t="s">
         <v>287</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E63" s="76"/>
-      <c r="F63" s="76"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="71"/>
       <c r="G63" s="59">
         <v>1</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J63" s="75" t="s">
+      <c r="J63" s="70" t="s">
         <v>60</v>
       </c>
       <c r="K63" s="18" t="b">
@@ -4489,21 +4499,21 @@
       <c r="B64" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C64" s="84" t="s">
+      <c r="C64" s="79" t="s">
         <v>290</v>
       </c>
       <c r="D64" s="63" t="s">
         <v>244</v>
       </c>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="71"/>
       <c r="G64" s="59">
         <v>1</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J64" s="75" t="s">
+      <c r="J64" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K64" s="18" t="b">
@@ -4526,14 +4536,14 @@
       <c r="B65" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C65" s="79" t="s">
+      <c r="C65" s="74" t="s">
         <v>292</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
       <c r="G65" s="59">
         <v>2</v>
       </c>
@@ -4543,7 +4553,7 @@
       <c r="I65" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J65" s="75" t="s">
+      <c r="J65" s="70" t="s">
         <v>293</v>
       </c>
       <c r="K65" s="18" t="b">
@@ -4567,14 +4577,14 @@
       <c r="B66" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C66" s="79" t="s">
+      <c r="C66" s="74" t="s">
         <v>295</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E66" s="76"/>
-      <c r="F66" s="76"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="71"/>
       <c r="G66" s="59">
         <v>2</v>
       </c>
@@ -4584,7 +4594,7 @@
       <c r="I66" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J66" s="75" t="s">
+      <c r="J66" s="70" t="s">
         <v>296</v>
       </c>
       <c r="K66" s="18" t="b">
@@ -4608,14 +4618,14 @@
       <c r="B67" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C67" s="79" t="s">
+      <c r="C67" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E67" s="76"/>
-      <c r="F67" s="76"/>
+      <c r="E67" s="71"/>
+      <c r="F67" s="71"/>
       <c r="G67" s="59">
         <v>6</v>
       </c>
@@ -4625,7 +4635,7 @@
       <c r="I67" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J67" s="75" t="s">
+      <c r="J67" s="70" t="s">
         <v>299</v>
       </c>
       <c r="K67" s="18" t="b">
@@ -4649,14 +4659,14 @@
       <c r="B68" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C68" s="79" t="s">
+      <c r="C68" s="74" t="s">
         <v>301</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
+      <c r="E68" s="71"/>
+      <c r="F68" s="71"/>
       <c r="G68" s="59">
         <v>6</v>
       </c>
@@ -4666,7 +4676,7 @@
       <c r="I68" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J68" s="75" t="s">
+      <c r="J68" s="70" t="s">
         <v>302</v>
       </c>
       <c r="K68" s="18" t="b">
@@ -4690,14 +4700,14 @@
       <c r="B69" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C69" s="79" t="s">
+      <c r="C69" s="74" t="s">
         <v>304</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
       <c r="G69" s="59">
         <v>6</v>
       </c>
@@ -4707,7 +4717,7 @@
       <c r="I69" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J69" s="75" t="s">
+      <c r="J69" s="70" t="s">
         <v>305</v>
       </c>
       <c r="K69" s="18" t="b">
@@ -4731,21 +4741,21 @@
       <c r="B70" s="60" t="s">
         <v>306</v>
       </c>
-      <c r="C70" s="82" t="s">
+      <c r="C70" s="77" t="s">
         <v>307</v>
       </c>
       <c r="D70" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
       <c r="G70" s="59">
         <v>2</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J70" s="75" t="s">
+      <c r="J70" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K70" s="20"/>
@@ -4765,14 +4775,14 @@
       <c r="B71" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C71" s="79" t="s">
+      <c r="C71" s="74" t="s">
         <v>309</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
+      <c r="E71" s="71"/>
+      <c r="F71" s="71"/>
       <c r="G71" s="59">
         <v>2</v>
       </c>
@@ -4782,7 +4792,7 @@
       <c r="I71" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="J71" s="75" t="s">
+      <c r="J71" s="70" t="s">
         <v>311</v>
       </c>
       <c r="K71" s="18" t="b">
@@ -4800,14 +4810,14 @@
       <c r="B72" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C72" s="79" t="s">
+      <c r="C72" s="74" t="s">
         <v>313</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
       <c r="G72" s="59">
         <v>14</v>
       </c>
@@ -4817,7 +4827,7 @@
       <c r="I72" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J72" s="75" t="s">
+      <c r="J72" s="70" t="s">
         <v>314</v>
       </c>
       <c r="K72" s="18" t="b">
@@ -4841,14 +4851,14 @@
       <c r="B73" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C73" s="79" t="s">
+      <c r="C73" s="74" t="s">
         <v>316</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
       <c r="G73" s="59">
         <v>2</v>
       </c>
@@ -4858,7 +4868,7 @@
       <c r="I73" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J73" s="75" t="s">
+      <c r="J73" s="70" t="s">
         <v>317</v>
       </c>
       <c r="K73" s="18" t="b">
@@ -4882,14 +4892,14 @@
       <c r="B74" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C74" s="79" t="s">
+      <c r="C74" s="74" t="s">
         <v>319</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
+      <c r="E74" s="71"/>
+      <c r="F74" s="71"/>
       <c r="G74" s="59">
         <v>2</v>
       </c>
@@ -4899,7 +4909,7 @@
       <c r="I74" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J74" s="75" t="s">
+      <c r="J74" s="70" t="s">
         <v>320</v>
       </c>
       <c r="K74" s="18" t="b">
@@ -4923,14 +4933,14 @@
       <c r="B75" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C75" s="79" t="s">
+      <c r="C75" s="74" t="s">
         <v>322</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
+      <c r="E75" s="71"/>
+      <c r="F75" s="71"/>
       <c r="G75" s="59">
         <v>6</v>
       </c>
@@ -4940,7 +4950,7 @@
       <c r="I75" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J75" s="75" t="s">
+      <c r="J75" s="70" t="s">
         <v>323</v>
       </c>
       <c r="K75" s="18" t="b">
@@ -4964,14 +4974,14 @@
       <c r="B76" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C76" s="79" t="s">
+      <c r="C76" s="74" t="s">
         <v>325</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
       <c r="G76" s="59">
         <v>4</v>
       </c>
@@ -4981,7 +4991,7 @@
       <c r="I76" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J76" s="75" t="s">
+      <c r="J76" s="70" t="s">
         <v>326</v>
       </c>
       <c r="K76" s="18" t="b">
@@ -5005,14 +5015,14 @@
       <c r="B77" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="C77" s="79" t="s">
+      <c r="C77" s="74" t="s">
         <v>328</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E77" s="76"/>
-      <c r="F77" s="76"/>
+      <c r="E77" s="71"/>
+      <c r="F77" s="71"/>
       <c r="G77" s="59">
         <v>2</v>
       </c>
@@ -5022,7 +5032,7 @@
       <c r="I77" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J77" s="75" t="s">
+      <c r="J77" s="70" t="s">
         <v>329</v>
       </c>
       <c r="K77" s="18" t="b">
@@ -5046,14 +5056,14 @@
       <c r="B78" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="C78" s="79" t="s">
+      <c r="C78" s="74" t="s">
         <v>331</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E78" s="76"/>
-      <c r="F78" s="76"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
       <c r="G78" s="59">
         <v>4</v>
       </c>
@@ -5063,7 +5073,7 @@
       <c r="I78" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J78" s="75" t="s">
+      <c r="J78" s="70" t="s">
         <v>332</v>
       </c>
       <c r="K78" s="18" t="b">
@@ -5087,21 +5097,21 @@
       <c r="B79" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C79" s="79" t="s">
+      <c r="C79" s="74" t="s">
         <v>334</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E79" s="76"/>
-      <c r="F79" s="76"/>
+      <c r="E79" s="71"/>
+      <c r="F79" s="71"/>
       <c r="G79" s="59">
         <v>8</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J79" s="75" t="s">
+      <c r="J79" s="70" t="s">
         <v>335</v>
       </c>
       <c r="K79" s="18" t="b">
@@ -5119,21 +5129,21 @@
       <c r="B80" s="61" t="s">
         <v>336</v>
       </c>
-      <c r="C80" s="83" t="s">
+      <c r="C80" s="78" t="s">
         <v>337</v>
       </c>
       <c r="D80" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="E80" s="76"/>
-      <c r="F80" s="76"/>
+      <c r="E80" s="71"/>
+      <c r="F80" s="71"/>
       <c r="G80" s="59">
         <v>1</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="J80" s="75" t="s">
+      <c r="J80" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K80" s="20"/>
@@ -5153,21 +5163,21 @@
       <c r="B81" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C81" s="79" t="s">
+      <c r="C81" s="74" t="s">
         <v>339</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E81" s="76"/>
-      <c r="F81" s="76"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
       <c r="G81" s="59">
         <v>1</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J81" s="75" t="s">
+      <c r="J81" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K81" s="18" t="b">
@@ -5185,21 +5195,21 @@
       <c r="B82" s="61" t="s">
         <v>340</v>
       </c>
-      <c r="C82" s="83" t="s">
+      <c r="C82" s="78" t="s">
         <v>341</v>
       </c>
       <c r="D82" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="E82" s="76"/>
-      <c r="F82" s="76"/>
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
       <c r="G82" s="59">
         <v>1</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J82" s="75" t="s">
+      <c r="J82" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K82" s="20"/>
@@ -5219,21 +5229,21 @@
       <c r="B83" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="C83" s="79" t="s">
+      <c r="C83" s="74" t="s">
         <v>343</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E83" s="76"/>
-      <c r="F83" s="76"/>
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
       <c r="G83" s="59">
         <v>1</v>
       </c>
       <c r="I83" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J83" s="75" t="s">
+      <c r="J83" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K83" s="18" t="b">
@@ -5253,21 +5263,21 @@
       <c r="B84" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="C84" s="79" t="s">
+      <c r="C84" s="74" t="s">
         <v>346</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E84" s="76"/>
-      <c r="F84" s="76"/>
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
       <c r="G84" s="59">
         <v>1</v>
       </c>
       <c r="I84" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J84" s="75" t="s">
+      <c r="J84" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K84" s="18" t="b">
@@ -5287,21 +5297,21 @@
       <c r="B85" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="C85" s="79" t="s">
+      <c r="C85" s="74" t="s">
         <v>348</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E85" s="76"/>
-      <c r="F85" s="76"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="71"/>
       <c r="G85" s="59">
         <v>1</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J85" s="75" t="s">
+      <c r="J85" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K85" s="18" t="b">
@@ -5321,21 +5331,21 @@
       <c r="B86" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="C86" s="81" t="s">
+      <c r="C86" s="76" t="s">
         <v>350</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="E86" s="76"/>
-      <c r="F86" s="76"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="71"/>
       <c r="G86" s="64">
         <v>1</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J86" s="75" t="s">
+      <c r="J86" s="70" t="s">
         <v>382</v>
       </c>
       <c r="K86" s="20"/>
@@ -5357,21 +5367,21 @@
       <c r="B87" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="C87" s="79" t="s">
+      <c r="C87" s="74" t="s">
         <v>354</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E87" s="76"/>
-      <c r="F87" s="76"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="71"/>
       <c r="G87" s="59">
         <v>1</v>
       </c>
       <c r="I87" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J87" s="75" t="s">
+      <c r="J87" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K87" s="18" t="b">
@@ -5391,21 +5401,21 @@
       <c r="B88" s="61" t="s">
         <v>355</v>
       </c>
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="78" t="s">
         <v>356</v>
       </c>
       <c r="D88" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="E88" s="76"/>
-      <c r="F88" s="76"/>
+      <c r="E88" s="71"/>
+      <c r="F88" s="71"/>
       <c r="G88" s="59">
         <v>1</v>
       </c>
       <c r="I88" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J88" s="75" t="s">
+      <c r="J88" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K88" s="20"/>
@@ -5424,14 +5434,14 @@
       <c r="B89" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="C89" s="79" t="s">
+      <c r="C89" s="74" t="s">
         <v>358</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
+      <c r="E89" s="71"/>
+      <c r="F89" s="71"/>
       <c r="G89" s="59">
         <v>1</v>
       </c>
@@ -5441,7 +5451,7 @@
       <c r="I89" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J89" s="75" t="s">
+      <c r="J89" s="70" t="s">
         <v>360</v>
       </c>
       <c r="K89" s="18" t="b">
@@ -5466,21 +5476,21 @@
       <c r="B90" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C90" s="79" t="s">
+      <c r="C90" s="74" t="s">
         <v>364</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E90" s="76"/>
-      <c r="F90" s="76"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="71"/>
       <c r="G90" s="59">
         <v>1</v>
       </c>
       <c r="I90" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J90" s="75" t="s">
+      <c r="J90" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K90" s="18" t="b">
@@ -5498,21 +5508,21 @@
       <c r="B91" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="C91" s="79" t="s">
+      <c r="C91" s="74" t="s">
         <v>366</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E91" s="76"/>
-      <c r="F91" s="76"/>
+      <c r="E91" s="71"/>
+      <c r="F91" s="71"/>
       <c r="G91" s="59">
         <v>1</v>
       </c>
       <c r="I91" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J91" s="75" t="s">
+      <c r="J91" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K91" s="18" t="b">
@@ -5530,21 +5540,21 @@
       <c r="B92" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C92" s="79" t="s">
+      <c r="C92" s="74" t="s">
         <v>368</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="E92" s="76"/>
-      <c r="F92" s="76"/>
+      <c r="E92" s="71"/>
+      <c r="F92" s="71"/>
       <c r="G92" s="59">
         <v>1</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J92" s="75" t="s">
+      <c r="J92" s="70" t="s">
         <v>245</v>
       </c>
       <c r="K92" s="18" t="b">
@@ -5570,8 +5580,8 @@
       <c r="D93" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E93" s="76"/>
-      <c r="F93" s="76"/>
+      <c r="E93" s="71"/>
+      <c r="F93" s="71"/>
       <c r="G93" s="64">
         <v>77</v>
       </c>
@@ -5581,7 +5591,7 @@
       <c r="I93" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J93" s="75" t="s">
+      <c r="J93" s="70" t="s">
         <v>371</v>
       </c>
       <c r="K93" s="22"/>
@@ -5608,8 +5618,8 @@
       <c r="D94" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E94" s="76"/>
-      <c r="F94" s="76"/>
+      <c r="E94" s="71"/>
+      <c r="F94" s="71"/>
       <c r="G94" s="64">
         <v>77</v>
       </c>
@@ -5619,7 +5629,7 @@
       <c r="I94" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J94" s="75" t="s">
+      <c r="J94" s="70" t="s">
         <v>374</v>
       </c>
       <c r="K94" s="22"/>
@@ -5646,8 +5656,8 @@
       <c r="D95" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E95" s="76"/>
-      <c r="F95" s="76"/>
+      <c r="E95" s="71"/>
+      <c r="F95" s="71"/>
       <c r="G95" s="64">
         <v>37</v>
       </c>
@@ -5657,7 +5667,7 @@
       <c r="I95" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J95" s="75" t="s">
+      <c r="J95" s="70" t="s">
         <v>377</v>
       </c>
       <c r="K95" s="22"/>
@@ -5684,8 +5694,8 @@
       <c r="D96" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E96" s="76"/>
-      <c r="F96" s="76"/>
+      <c r="E96" s="71"/>
+      <c r="F96" s="71"/>
       <c r="G96" s="59">
         <v>37</v>
       </c>
@@ -5695,7 +5705,7 @@
       <c r="I96" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J96" s="75" t="s">
+      <c r="J96" s="70" t="s">
         <v>380</v>
       </c>
       <c r="K96" s="22"/>
@@ -6464,74 +6474,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="74"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="29" t="s">
@@ -6578,22 +6588,22 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="31">
@@ -6685,22 +6695,22 @@
       <c r="L9" s="22"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="40" t="s">
@@ -6814,22 +6824,22 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="31">
@@ -6889,22 +6899,22 @@
       <c r="N19" s="38"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
-      <c r="J20" s="70"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="70"/>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="40" t="s">
@@ -7104,19 +7114,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:Y54"/>
+  <dimension ref="A3:Y55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" ht="12.75">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7130,55 +7142,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="38.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="86" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" ht="51">
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" ht="12.75">
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="86" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" customHeight="1">
+      <c r="C7" s="67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="12.75">
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -7186,32 +7205,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" ht="12.75">
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" ht="12.75">
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" ht="12.75">
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" ht="12.75">
       <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" ht="12.75">
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" ht="12.75">
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
@@ -7221,297 +7240,285 @@
         <v>394</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
-      <c r="B18" s="2" t="s">
+    <row r="17" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1">
+      <c r="C17" s="53" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="12.75">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="14" t="str">
+      <c r="E19" s="14" t="str">
         <f>HYPERLINK("https://www.ponoko.com/","Ponoko")</f>
         <v>Ponoko</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
-      <c r="C19" s="3" t="s">
+    <row r="20" spans="1:25" ht="12.75">
+      <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="19" t="s">
+    <row r="21" spans="1:25" ht="12.75">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" ht="12.75">
+      <c r="A22" s="17"/>
+      <c r="B22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:25" ht="12.75">
+      <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="1:25" ht="12.75">
+      <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E24" s="3">
         <v>2</v>
       </c>
-      <c r="F23" s="3">
-        <f>3+SUM(F34)+SUM(F41,F42)+F46</f>
+      <c r="F24" s="3">
+        <f>3+SUM(F35)+SUM(F42,F43)+F47</f>
         <v>8</v>
       </c>
-      <c r="G23" s="3">
-        <f>2+SUM(F32,F33,F35)+SUM(F43)</f>
+      <c r="G24" s="3">
+        <f>2+SUM(F33,F34,F36)+SUM(F44)</f>
         <v>10</v>
       </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
-      <c r="C24" s="5" t="s">
+    <row r="25" spans="1:25" ht="12.75">
+      <c r="C25" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="25">
-        <f>F38</f>
+      <c r="F25" s="25">
+        <f>F39</f>
         <v>1</v>
       </c>
-      <c r="G24" s="25">
-        <f>F51+F54</f>
+      <c r="G25" s="25">
+        <f>F52+F55</f>
         <v>3</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H25" s="3">
         <v>2</v>
       </c>
-      <c r="J24" s="3">
-        <f>F50+F49</f>
+      <c r="J25" s="3">
+        <f>F51+F50</f>
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
-      <c r="C25" s="5" t="s">
+    <row r="26" spans="1:25" ht="12.75">
+      <c r="C26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="3">
-        <f>1+F54</f>
+      <c r="G26" s="3">
+        <f>1+F55</f>
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
-      <c r="C26" s="5" t="s">
+    <row r="27" spans="1:25" ht="12.75">
+      <c r="C27" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="25">
-        <f>F53+F52</f>
+      <c r="J27" s="25">
+        <f>F54+F53</f>
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="19" t="s">
+    <row r="30" spans="1:25" ht="12.75">
+      <c r="A30" s="27"/>
+      <c r="B30" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-    </row>
-    <row r="31" spans="1:25">
-      <c r="B31" s="2" t="s">
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+    </row>
+    <row r="32" spans="1:25" ht="12.75">
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="1" t="s">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="2:6" ht="12.75">
+      <c r="B33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E33" s="25">
         <f>ROUNDUP(467/25.4,2)</f>
         <v>18.39</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F33" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="3" t="s">
+    <row r="34" spans="2:6" ht="12.75">
+      <c r="B34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E34" s="25">
         <f>ROUNDUP(442/25.4,2)</f>
         <v>17.41</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F34" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="3" t="s">
+    <row r="35" spans="2:6" ht="12.75">
+      <c r="B35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E35" s="25">
         <f>ROUNDUP(254.8/25.4,2)</f>
         <v>10.039999999999999</v>
       </c>
-      <c r="F34" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="25">
-        <f t="shared" ref="E35:E36" si="0">ROUNDUP(558.8/25.4,2)</f>
-        <v>22</v>
-      </c>
       <c r="F35" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="5" t="s">
+    <row r="36" spans="2:6" ht="12.75">
+      <c r="B36" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="25">
+        <f t="shared" ref="E36:E37" si="0">ROUNDUP(558.8/25.4,2)</f>
+        <v>22</v>
+      </c>
+      <c r="F36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="12.75">
+      <c r="B37" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E37" s="25">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F37" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="2:6" ht="12.75">
+      <c r="B38" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="3">
-        <v>36</v>
-      </c>
-      <c r="F37" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>64</v>
@@ -7519,237 +7526,254 @@
       <c r="D38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="3">
+        <v>36</v>
+      </c>
+      <c r="F38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="12.75">
+      <c r="B39" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="25">
         <f>ROUNDUP(241/25.4,2)</f>
         <v>9.49</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F39" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
-      <c r="B40" s="1" t="s">
+    <row r="41" spans="2:6" ht="12.75">
+      <c r="B41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="1" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="5" t="s">
+    <row r="42" spans="2:6" ht="12.75">
+      <c r="B42" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E42" s="25">
         <f>ROUNDUP(200.2/25.4,2)</f>
         <v>7.89</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F42" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="5" t="s">
+    <row r="43" spans="2:6" ht="12.75">
+      <c r="B43" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E43" s="25">
         <f>ROUNDUP(251/25.4,2)</f>
         <v>9.89</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F43" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="2:6" ht="12.75">
+      <c r="B44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E44" s="25">
         <f>ROUNDUP(391/25.4,2)</f>
         <v>15.4</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F44" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="2:6" ht="12.75">
+      <c r="B46" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="1" t="s">
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="3" t="s">
+    <row r="47" spans="2:6" ht="12.75">
+      <c r="B47" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E47" s="25">
         <f>ROUNDUP(304.8/25.4,2)</f>
         <v>12</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F47" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="2:6" ht="12.75">
+      <c r="B49" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="1" t="s">
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
-      <c r="B49" s="3" t="s">
+    <row r="50" spans="2:6" ht="12.75">
+      <c r="B50" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E50" s="25">
         <f>ROUNDUP(1908/25.4,2)</f>
         <v>75.12</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F50" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
-      <c r="B50" s="3" t="s">
+    <row r="51" spans="2:6" ht="12.75">
+      <c r="B51" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E51" s="25">
         <f>ROUNDUP(2057.4/25.4,2)</f>
         <v>81</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F51" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
-      <c r="B51" s="5" t="s">
+    <row r="52" spans="2:6" ht="12.75">
+      <c r="B52" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E52" s="25">
         <f>ROUNDUP(583.4/25.4,2)</f>
         <v>22.970000000000002</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F52" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
-      <c r="B52" s="3" t="s">
+    <row r="53" spans="2:6" ht="12.75">
+      <c r="B53" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E53" s="25">
         <f>ROUNDUP(1908/25.4,2)</f>
         <v>75.12</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F53" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="2:6" ht="12.75">
+      <c r="B54" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E54" s="25">
         <f>ROUNDUP(2057.4/25.4,2)</f>
         <v>81</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F54" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="3" t="s">
+    <row r="55" spans="2:6" ht="12.75">
+      <c r="B55" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E55" s="25">
         <f>ROUNDUP(604.8/25.4,2)</f>
         <v>23.82</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F55" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D18" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D19" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D20" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>